<commit_message>
Fix error in SystemB soil. Tidying.
</commit_message>
<xml_diff>
--- a/Tests/Simulation/SoilNitrogenPatch/Ep Speed.xlsx
+++ b/Tests/Simulation/SoilNitrogenPatch/Ep Speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaUnderVC\ApsimNextGen\Tests\Simulation\SoilNitrogenPatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B458FBE-54FB-4B2D-ABA8-53A83A246C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85767B66-5395-4CD5-96A6-24B22E971BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="180" windowWidth="28275" windowHeight="19260" xr2:uid="{A4FEE623-5290-4DFF-8806-D3DF43719108}"/>
+    <workbookView xWindow="24345" yWindow="2625" windowWidth="23160" windowHeight="18225" xr2:uid="{A4FEE623-5290-4DFF-8806-D3DF43719108}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Patches</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Hours for a 45-year sim</t>
+  </si>
+  <si>
+    <t>, 5,10, 50,100, 500</t>
   </si>
 </sst>
 </file>
@@ -1865,15 +1868,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EA39C9-58E6-46B1-91E4-B83B8A935A9A}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1915,8 +1918,11 @@
         <f>D2/A2/B2</f>
         <v>0.49</v>
       </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -1942,7 +1948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>0.188</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>0.24640000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -2011,7 +2017,7 @@
         <v>0.41194999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>0.93628</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2090,8 +2096,12 @@
         <f t="shared" ref="K9:K14" si="5">E9/60*45/5</f>
         <v>2.5000000000000001E-3</v>
       </c>
+      <c r="M9">
+        <f>6*K9</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>3.5650000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -2152,8 +2162,12 @@
         <f t="shared" si="5"/>
         <v>0.118725</v>
       </c>
+      <c r="M11">
+        <f>6*K11</f>
+        <v>0.71235000000000004</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -2183,8 +2197,12 @@
         <f t="shared" si="5"/>
         <v>0.24554999999999999</v>
       </c>
+      <c r="M12">
+        <f>6*K12</f>
+        <v>1.4733000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>200</v>
       </c>
@@ -2215,7 +2233,7 @@
         <v>0.71069999999999989</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>500</v>
       </c>
@@ -2245,8 +2263,12 @@
         <f t="shared" si="5"/>
         <v>4.0032249999999996</v>
       </c>
+      <c r="M14">
+        <f>6*K14</f>
+        <v>24.019349999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1000</v>
       </c>

</xml_diff>